<commit_message>
Elise runs through example code
</commit_message>
<xml_diff>
--- a/data/hyde_park_points.xlsx
+++ b/data/hyde_park_points.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisegallois/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisegallois/Desktop/microclima_tutorial/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82BDDCE6-5C44-6F43-B6E7-69D3DE3B7547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED74C10-8361-5D4D-B826-F6FBC96CC68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="500" windowWidth="21600" windowHeight="16680" xr2:uid="{83469B59-F4BF-6D42-8E02-D04C52868BCE}"/>
+    <workbookView xWindow="6820" yWindow="500" windowWidth="21600" windowHeight="16620" xr2:uid="{83469B59-F4BF-6D42-8E02-D04C52868BCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,12 +456,12 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -469,10 +469,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.45">
@@ -480,87 +480,87 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
+        <v>-0.1641</v>
+      </c>
+      <c r="C2" s="1">
         <v>51.507399999999997</v>
-      </c>
-      <c r="C2" s="1">
-        <v>-0.1641</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
+        <v>-0.1663</v>
+      </c>
+      <c r="C3" s="1">
         <v>51.505400000000002</v>
-      </c>
-      <c r="C3">
-        <v>-0.1663</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
+        <v>-0.1653</v>
+      </c>
+      <c r="C4" s="1">
         <v>51.506399999999999</v>
-      </c>
-      <c r="C4">
-        <v>-0.1653</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
+        <v>-0.1696</v>
+      </c>
+      <c r="C5" s="1">
         <v>51.5047</v>
-      </c>
-      <c r="C5">
-        <v>-0.1696</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
+        <v>-0.18165999999999999</v>
+      </c>
+      <c r="C6" s="1">
         <v>51.504899999999999</v>
-      </c>
-      <c r="C6">
-        <v>-0.18165999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
+        <v>-0.182671</v>
+      </c>
+      <c r="C7" s="1">
         <v>51.509686000000002</v>
-      </c>
-      <c r="C7">
-        <v>-0.182671</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
+        <v>-0.15853500000000001</v>
+      </c>
+      <c r="C8" s="1">
         <v>51.509101000000001</v>
-      </c>
-      <c r="C8">
-        <v>-0.15853500000000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
+        <v>-0.15312400000000001</v>
+      </c>
+      <c r="C9" s="1">
         <v>51.503757</v>
-      </c>
-      <c r="C9">
-        <v>-0.15312400000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>